<commit_message>
- Added languages template xlsx file
</commit_message>
<xml_diff>
--- a/public/files/templates/import_langs.xlsx
+++ b/public/files/templates/import_langs.xlsx
@@ -1,50 +1,71 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646470D2-DEAC-4AA5-8154-9F934E0FA418}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A63D53-4C69-4435-9219-F4D38390A42A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>finished_reading_date</t>
-  </si>
-  <si>
-    <t>publish_year</t>
-  </si>
-  <si>
-    <t>Author test 1</t>
-  </si>
-  <si>
-    <t>Author test 2</t>
-  </si>
-  <si>
-    <t>Title test 1</t>
-  </si>
-  <si>
-    <t>Title test 2</t>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>native</t>
+  </si>
+  <si>
+    <t>native_en</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>fg</t>
+  </si>
+  <si>
+    <t>Fagan</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>2018-07-29 10:27:49</t>
+  </si>
+  <si>
+    <t>2018-07-29 10:58:07</t>
+  </si>
+  <si>
+    <t>2018-07-29 10:27:50</t>
+  </si>
+  <si>
+    <t>2018-07-29 10:58:08</t>
+  </si>
+  <si>
+    <t>Datan</t>
+  </si>
+  <si>
+    <t>en</t>
   </si>
 </sst>
 </file>
@@ -60,11 +81,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -76,12 +95,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -89,81 +108,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -499,73 +466,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="4"/>
-    <col min="2" max="2" width="35" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.88671875" style="4" customWidth="1"/>
-    <col min="4" max="6" width="36.33203125" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="14.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6">
-        <v>43101</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6">
-        <v>43132</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Replaced langauges template file with empty XLSX template file
</commit_message>
<xml_diff>
--- a/public/files/templates/import_langs.xlsx
+++ b/public/files/templates/import_langs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A63D53-4C69-4435-9219-F4D38390A42A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9774C49-C518-4DCF-B420-8A77D60A9AB2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
@@ -39,33 +39,6 @@
   </si>
   <si>
     <t>updated_at</t>
-  </si>
-  <si>
-    <t>fg</t>
-  </si>
-  <si>
-    <t>Fagan</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>2018-07-29 10:27:49</t>
-  </si>
-  <si>
-    <t>2018-07-29 10:58:07</t>
-  </si>
-  <si>
-    <t>2018-07-29 10:27:50</t>
-  </si>
-  <si>
-    <t>2018-07-29 10:58:08</t>
-  </si>
-  <si>
-    <t>Datan</t>
-  </si>
-  <si>
-    <t>en</t>
   </si>
 </sst>
 </file>
@@ -113,7 +86,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -123,9 +96,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -466,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,58 +481,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>